<commit_message>
test Rajout dossier Scripts + modif Gantt
</commit_message>
<xml_diff>
--- a/Presentations/gantt.xlsx
+++ b/Presentations/gantt.xlsx
@@ -32,9 +32,6 @@
     <t>Début</t>
   </si>
   <si>
-    <t>Durée (semaines)</t>
-  </si>
-  <si>
     <t>16 semaines</t>
   </si>
   <si>
@@ -55,11 +52,17 @@
   <si>
     <t>Tests et debugging</t>
   </si>
+  <si>
+    <t>Durée (jours)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="d/m;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -239,25 +243,25 @@
             <c:numRef>
               <c:f>Feuil1!$C$3:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>d/m;@</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>41654</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>41623</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>41636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>41593</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>41593</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>41579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -272,7 +276,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Durée (semaines)</c:v>
+                  <c:v>Durée (jours)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -320,22 +324,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,11 +355,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="159211664"/>
-        <c:axId val="159216760"/>
+        <c:axId val="146715856"/>
+        <c:axId val="146714288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="159211664"/>
+        <c:axId val="146715856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +402,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="159216760"/>
+        <c:crossAx val="146714288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -406,11 +410,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159216760"/>
+        <c:axId val="146714288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="17"/>
-          <c:min val="0"/>
+          <c:max val="41689"/>
+          <c:min val="41578"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -428,7 +432,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="d/m;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -459,9 +463,10 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="159211664"/>
+        <c:crossAx val="146715856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="15"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1093,16 +1098,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2490787</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1387,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1407,80 +1412,111 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>14</v>
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>41654</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>41623</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>41636</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>41593</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>41593</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1">
+        <v>41579</v>
+      </c>
+      <c r="D8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
         <v>0</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Unity - Serialisation + Classes
Attention : les constructeurs sont remplis de manière bidon.
</commit_message>
<xml_diff>
--- a/Presentations/gantt.xlsx
+++ b/Presentations/gantt.xlsx
@@ -61,7 +61,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="d/m;@"/>
+    <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -94,7 +94,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -333,10 +333,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14</c:v>
@@ -355,11 +355,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="146715856"/>
-        <c:axId val="146714288"/>
+        <c:axId val="199406424"/>
+        <c:axId val="199401720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146715856"/>
+        <c:axId val="199406424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,7 +402,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146714288"/>
+        <c:crossAx val="199401720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -410,7 +410,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="146714288"/>
+        <c:axId val="199401720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41689"/>
@@ -463,7 +463,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146715856"/>
+        <c:crossAx val="199406424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="15"/>
@@ -1099,15 +1099,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>223837</xdr:colOff>
+      <xdr:colOff>33337</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1395,7 +1395,7 @@
   <dimension ref="B2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,7 +1459,7 @@
         <v>41593</v>
       </c>
       <c r="D6">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
         <v>41593</v>
       </c>
       <c r="D7">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>